<commit_message>
feat - ajustado classe planilha para funcionar com openpyxl
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Apresentação" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Planejamento Tributário" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="CNPJ">Apresentação!$C$7</definedName>
+    <definedName name="EMPRESA">Apresentação!$B$7</definedName>
+  </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -287,7 +290,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
@@ -414,10 +417,13 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -776,48 +782,53 @@
   </sheetPr>
   <dimension ref="A7:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="84.42578125" customWidth="1" style="97" min="2" max="2"/>
-    <col width="16" customWidth="1" style="97" min="3" max="3"/>
-    <col width="8.5703125" customWidth="1" style="97" min="4" max="4"/>
-    <col width="11.42578125" customWidth="1" style="97" min="5" max="5"/>
-    <col width="16.5703125" bestFit="1" customWidth="1" style="97" min="6" max="6"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="97" min="7" max="7"/>
+    <col width="84.42578125" customWidth="1" style="96" min="2" max="2"/>
+    <col width="16" customWidth="1" style="96" min="3" max="3"/>
+    <col width="8.5703125" customWidth="1" style="96" min="4" max="4"/>
+    <col width="11.42578125" customWidth="1" style="96" min="5" max="5"/>
+    <col width="16.5703125" bestFit="1" customWidth="1" style="96" min="6" max="6"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="96" min="7" max="7"/>
     <col width="8.85546875" customWidth="1" style="50" min="9" max="9"/>
-    <col width="15.5703125" bestFit="1" customWidth="1" style="97" min="10" max="10"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" style="96" min="10" max="10"/>
     <col width="8.7109375" customWidth="1" style="60" min="11" max="11"/>
-    <col width="11.85546875" bestFit="1" customWidth="1" style="97" min="12" max="12"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" style="96" min="12" max="12"/>
     <col width="2.85546875" bestFit="1" customWidth="1" style="60" min="13" max="13"/>
     <col width="19.140625" bestFit="1" customWidth="1" style="60" min="14" max="14"/>
-    <col width="14.5703125" customWidth="1" style="97" min="15" max="15"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="97" min="16" max="16"/>
-    <col width="7.85546875" bestFit="1" customWidth="1" style="97" min="18" max="18"/>
-    <col width="10.140625" bestFit="1" customWidth="1" style="97" min="19" max="19"/>
-    <col width="17.5703125" bestFit="1" customWidth="1" style="97" min="16377" max="16377"/>
-    <col width="16.140625" bestFit="1" customWidth="1" style="97" min="16378" max="16379"/>
-    <col width="10.5703125" bestFit="1" customWidth="1" style="97" min="16382" max="16382"/>
+    <col width="14.5703125" customWidth="1" style="96" min="15" max="15"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="96" min="16" max="16"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="96" min="18" max="18"/>
+    <col width="10.140625" bestFit="1" customWidth="1" style="96" min="19" max="19"/>
+    <col width="17.5703125" bestFit="1" customWidth="1" style="96" min="16377" max="16377"/>
+    <col width="16.140625" bestFit="1" customWidth="1" style="96" min="16378" max="16379"/>
+    <col width="10.5703125" bestFit="1" customWidth="1" style="96" min="16382" max="16382"/>
   </cols>
   <sheetData>
     <row r="7">
       <c r="A7" s="52" t="n"/>
       <c r="B7" s="49" t="inlineStr">
         <is>
-          <t>EMPRESA: Teste</t>
+          <t>EMPRESA: Empresa ABC</t>
+        </is>
+      </c>
+      <c r="C7" s="98" t="inlineStr">
+        <is>
+          <t>CNPJ: 00.111.222/0001-03</t>
         </is>
       </c>
       <c r="D7" s="52" t="inlineStr">
         <is>
-          <t>CNPJ: 12345678901234</t>
+          <t>CNPJ: 123456789</t>
         </is>
       </c>
       <c r="H7" s="2" t="n"/>
     </row>
-    <row r="10" ht="21" customHeight="1" s="97">
+    <row r="10" ht="21" customHeight="1" s="96">
       <c r="B10" s="42" t="inlineStr">
         <is>
           <t>Resumo Tributário: Simples Nacional</t>
@@ -829,7 +840,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1" s="97" thickBot="1"/>
+    <row r="11" ht="15.75" customHeight="1" s="96" thickBot="1"/>
     <row r="12">
       <c r="B12" s="13" t="inlineStr">
         <is>
@@ -895,7 +906,7 @@
       <c r="H14" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="J14" s="98" t="n"/>
+      <c r="J14" s="99" t="n"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>PIS</t>
@@ -922,7 +933,7 @@
       <c r="H15" s="18" t="n">
         <v>5</v>
       </c>
-      <c r="J15" s="98" t="n"/>
+      <c r="J15" s="99" t="n"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>COFINS</t>
@@ -961,7 +972,7 @@
     </row>
     <row r="17">
       <c r="B17" s="10" t="n"/>
-      <c r="F17" s="96" t="n"/>
+      <c r="F17" s="97" t="n"/>
       <c r="G17" s="11" t="n"/>
       <c r="H17" s="12" t="n"/>
       <c r="O17" t="inlineStr">
@@ -1017,7 +1028,7 @@
       <c r="H19" s="18" t="n">
         <v>14</v>
       </c>
-      <c r="J19" s="99" t="n"/>
+      <c r="J19" s="100" t="n"/>
       <c r="N19" s="82" t="n"/>
       <c r="O19" s="83" t="inlineStr">
         <is>
@@ -1054,7 +1065,7 @@
           <t>Compras</t>
         </is>
       </c>
-      <c r="O20" s="100">
+      <c r="O20" s="101">
         <f>(P16-O24)</f>
         <v/>
       </c>
@@ -1114,7 +1125,7 @@
           <t>Vendas</t>
         </is>
       </c>
-      <c r="P22" s="101">
+      <c r="P22" s="102">
         <f>(P18-P24)</f>
         <v/>
       </c>
@@ -1123,12 +1134,12 @@
           <t>PIS</t>
         </is>
       </c>
-      <c r="S22" s="102">
+      <c r="S22" s="103">
         <f>(P23*P14)-(O23*P14)</f>
         <v/>
       </c>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="97">
+    <row r="23" ht="18.75" customHeight="1" s="96">
       <c r="B23" s="10" t="inlineStr">
         <is>
           <t>IRPJ</t>
@@ -1152,11 +1163,11 @@
           <t>Base de Cálculo</t>
         </is>
       </c>
-      <c r="O23" s="103">
+      <c r="O23" s="104">
         <f>SUM(O20:O22)</f>
         <v/>
       </c>
-      <c r="P23" s="104">
+      <c r="P23" s="105">
         <f>SUM(P22)</f>
         <v/>
       </c>
@@ -1165,7 +1176,7 @@
           <t>COFINS</t>
         </is>
       </c>
-      <c r="S23" s="102">
+      <c r="S23" s="103">
         <f>(P23*P15)-(O23*P15)</f>
         <v/>
       </c>
@@ -1195,11 +1206,11 @@
           <t>Exclusão ICMS</t>
         </is>
       </c>
-      <c r="O24" s="105">
+      <c r="O24" s="106">
         <f>P16*P12</f>
         <v/>
       </c>
-      <c r="P24" s="106">
+      <c r="P24" s="107">
         <f>P18*P13</f>
         <v/>
       </c>
@@ -1268,7 +1279,7 @@
       <c r="H27" s="77" t="n">
         <v>0.17</v>
       </c>
-      <c r="J27" s="99" t="n"/>
+      <c r="J27" s="100" t="n"/>
       <c r="K27" s="74" t="n"/>
       <c r="L27" s="58" t="n"/>
       <c r="M27" s="74" t="n"/>
@@ -1302,7 +1313,7 @@
           <t>Custo Fixo - Teórico</t>
         </is>
       </c>
-      <c r="C30" s="107">
+      <c r="C30" s="108">
         <f>F30/16</f>
         <v/>
       </c>
@@ -1329,7 +1340,7 @@
           <t>Lucro - Teórico</t>
         </is>
       </c>
-      <c r="C31" s="107">
+      <c r="C31" s="108">
         <f>F31/16</f>
         <v/>
       </c>
@@ -1348,7 +1359,7 @@
       </c>
       <c r="H31" s="12" t="n"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="32" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="B32" s="27" t="inlineStr">
         <is>
           <t>TOTAL CARGA TRIBUTÁRIA</t>
@@ -1364,7 +1375,7 @@
       </c>
       <c r="H32" s="30" t="n"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="33" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="F33" s="1" t="n"/>
       <c r="G33" s="11" t="n"/>
     </row>
@@ -1408,7 +1419,7 @@
       <c r="H36" s="61" t="n">
         <v>0.01617920778151936</v>
       </c>
-      <c r="L36" s="96" t="n"/>
+      <c r="L36" s="97" t="n"/>
     </row>
     <row r="37">
       <c r="B37" s="10" t="inlineStr">
@@ -1427,7 +1438,7 @@
       <c r="H37" s="61" t="n">
         <v>0.076</v>
       </c>
-      <c r="L37" s="99" t="n"/>
+      <c r="L37" s="100" t="n"/>
     </row>
     <row r="38">
       <c r="B38" s="10" t="inlineStr">
@@ -1547,7 +1558,7 @@
       <c r="G46" s="11" t="n"/>
       <c r="H46" s="12" t="n"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="47" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="B47" s="53" t="inlineStr">
         <is>
           <t>% TRIBUTOS SOBRE O FATURAMENTO</t>
@@ -1566,7 +1577,7 @@
       </c>
       <c r="H47" s="56" t="n"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="48" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="B48" s="65" t="n"/>
       <c r="C48" s="65" t="n"/>
       <c r="D48" s="65" t="n"/>
@@ -1653,7 +1664,7 @@
       </c>
       <c r="H54" s="12" t="n"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="55" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="B55" s="38" t="inlineStr">
         <is>
           <t>Cofins</t>
@@ -1687,20 +1698,20 @@
       <c r="D60" s="11" t="n"/>
     </row>
     <row r="65">
-      <c r="B65" s="96" t="inlineStr">
+      <c r="B65" s="97" t="inlineStr">
         <is>
           <t>Tributação Presumido x Real</t>
         </is>
       </c>
     </row>
-    <row r="66" ht="11.45" customHeight="1" s="97">
+    <row r="66" ht="11.45" customHeight="1" s="96">
       <c r="B66" t="inlineStr">
         <is>
           <t>Impostos:</t>
         </is>
       </c>
     </row>
-    <row r="67" ht="18.95" customHeight="1" s="97">
+    <row r="67" ht="18.95" customHeight="1" s="96">
       <c r="B67" t="inlineStr">
         <is>
           <t>Folha</t>
@@ -1708,28 +1719,28 @@
       </c>
       <c r="C67" s="5" t="n"/>
     </row>
-    <row r="68" ht="17.45" customHeight="1" s="97">
+    <row r="68" ht="17.45" customHeight="1" s="96">
       <c r="B68" t="inlineStr">
         <is>
           <t>ICMS</t>
         </is>
       </c>
     </row>
-    <row r="69" ht="21.95" customHeight="1" s="97">
+    <row r="69" ht="21.95" customHeight="1" s="96">
       <c r="B69" t="inlineStr">
         <is>
           <t>IPI</t>
         </is>
       </c>
     </row>
-    <row r="70" ht="21" customHeight="1" s="97">
+    <row r="70" ht="21" customHeight="1" s="96">
       <c r="B70" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
     </row>
-    <row r="71" ht="21.6" customHeight="1" s="97">
+    <row r="71" ht="21.6" customHeight="1" s="96">
       <c r="B71" t="inlineStr">
         <is>
           <t>COFINS</t>
@@ -1753,38 +1764,36 @@
   </sheetPr>
   <dimension ref="B7:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29:N37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="32.5703125" bestFit="1" customWidth="1" style="97" min="2" max="2"/>
-    <col width="11.42578125" bestFit="1" customWidth="1" style="97" min="3" max="3"/>
-    <col width="11.42578125" customWidth="1" style="97" min="5" max="5"/>
-    <col width="11.42578125" bestFit="1" customWidth="1" style="97" min="6" max="6"/>
+    <col width="32.5703125" bestFit="1" customWidth="1" style="96" min="2" max="2"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" style="96" min="3" max="3"/>
+    <col width="11.42578125" customWidth="1" style="96" min="5" max="5"/>
+    <col width="11.42578125" bestFit="1" customWidth="1" style="96" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="7">
-      <c r="B7" s="49" t="inlineStr">
-        <is>
-          <t>Empresa: NOME EMPRESA LTDA</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CNPJ: 16.684.262/0001-52</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="21" customHeight="1" s="97">
+      <c r="B7" s="49">
+        <f>EMPRESA</f>
+        <v/>
+      </c>
+      <c r="D7" s="98">
+        <f>CNPJ</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" ht="21" customHeight="1" s="96">
       <c r="B10" s="42" t="inlineStr">
         <is>
           <t>Planejamento Tributário: Oportunidades Lucro Presumido x Lucro Real</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="15.75" customHeight="1" s="97" thickBot="1"/>
+    <row r="11" ht="15.75" customHeight="1" s="96" thickBot="1"/>
     <row r="12">
       <c r="B12" s="13" t="inlineStr">
         <is>
@@ -2017,7 +2026,7 @@
       </c>
       <c r="H28" s="12" t="n"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="29" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="B29" s="27" t="inlineStr">
         <is>
           <t>% TRIBUTOS SOBRE O FATURAMENTO</t>
@@ -2033,7 +2042,7 @@
       </c>
       <c r="H29" s="30" t="n"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="30" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="F30" s="1" t="n"/>
       <c r="G30" s="11" t="n"/>
     </row>
@@ -2187,7 +2196,7 @@
       </c>
       <c r="H42" s="12" t="n"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1" s="97" thickBot="1">
+    <row r="43" ht="15.75" customHeight="1" s="96" thickBot="1">
       <c r="B43" s="38" t="inlineStr">
         <is>
           <t>Cofins</t>
@@ -2251,20 +2260,20 @@
       </c>
     </row>
     <row r="53">
-      <c r="B53" s="96" t="inlineStr">
+      <c r="B53" s="97" t="inlineStr">
         <is>
           <t>Tributação Presumido x Real</t>
         </is>
       </c>
     </row>
-    <row r="54" ht="11.45" customHeight="1" s="97">
+    <row r="54" ht="11.45" customHeight="1" s="96">
       <c r="B54" t="inlineStr">
         <is>
           <t>Impostos:</t>
         </is>
       </c>
     </row>
-    <row r="55" ht="18.95" customHeight="1" s="97">
+    <row r="55" ht="18.95" customHeight="1" s="96">
       <c r="B55" t="inlineStr">
         <is>
           <t>Folha</t>
@@ -2272,28 +2281,28 @@
       </c>
       <c r="C55" s="5" t="n"/>
     </row>
-    <row r="56" ht="17.45" customHeight="1" s="97">
+    <row r="56" ht="17.45" customHeight="1" s="96">
       <c r="B56" t="inlineStr">
         <is>
           <t>ICMS</t>
         </is>
       </c>
     </row>
-    <row r="57" ht="21.95" customHeight="1" s="97">
+    <row r="57" ht="21.95" customHeight="1" s="96">
       <c r="B57" t="inlineStr">
         <is>
           <t>IPI</t>
         </is>
       </c>
     </row>
-    <row r="58" ht="21" customHeight="1" s="97">
+    <row r="58" ht="21" customHeight="1" s="96">
       <c r="B58" t="inlineStr">
         <is>
           <t>PIS</t>
         </is>
       </c>
     </row>
-    <row r="59" ht="21.6" customHeight="1" s="97">
+    <row r="59" ht="21.6" customHeight="1" s="96">
       <c r="B59" t="inlineStr">
         <is>
           <t>COFINS</t>

</xml_diff>

<commit_message>
bugfix - corrigido banner nao aparecia no output
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -513,6 +513,98 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <to>
+      <col>8</col>
+      <colOff>108405</colOff>
+      <row>5</row>
+      <rowOff>59690</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Imagem 6"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="11865429" cy="947964"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <to>
+      <col>8</col>
+      <colOff>273685</colOff>
+      <row>5</row>
+      <rowOff>63500</rowOff>
+    </to>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Imagem 6"/>
+        <cNvPicPr>
+          <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
+        </cNvPicPr>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="7369810" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -818,14 +910,10 @@
       </c>
       <c r="C7" s="98" t="inlineStr">
         <is>
-          <t>CNPJ: 00.111.222/0001-03</t>
-        </is>
-      </c>
-      <c r="D7" s="52" t="inlineStr">
-        <is>
           <t>CNPJ: 123456789</t>
         </is>
       </c>
+      <c r="D7" s="52" t="n"/>
       <c r="H7" s="2" t="n"/>
     </row>
     <row r="10" ht="21" customHeight="1" s="96">
@@ -1753,6 +1841,7 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9" scale="39"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2315,5 +2404,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
   <pageSetup orientation="portrait" paperSize="9" scale="63"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>